<commit_message>
added drop down spinner for venues and drawrect method to draw a bubble for when the venue is selected in the spinner
</commit_message>
<xml_diff>
--- a/Blair/Efforts_Logbook_Blair.xlsx
+++ b/Blair/Efforts_Logbook_Blair.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t xml:space="preserve">Your Name</t>
   </si>
@@ -137,6 +137,12 @@
     <t xml:space="preserve">Sprint # 6</t>
   </si>
   <si>
+    <t xml:space="preserve">attended team meetings, worked on live navigation features and shortest path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NavigineFragment.java</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint # 7</t>
   </si>
   <si>
@@ -209,7 +215,9 @@
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">Joe, Smith</t>
+    <t xml:space="preserve">Since this is named count I assume this keeps track of the count of things while the project progresses, however it does not make sense to me to have 5 E’s on sprint
+zero unless there are 5 things that were worked on that pertain to E. My assumption is that it keeps a running tally and that for each sprint, no matter how many things
+ I worked on if it fills a category, there will be one increment for the letter in question. Regardless, our independent work is self evident. </t>
   </si>
 </sst>
 </file>
@@ -220,7 +228,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -266,6 +274,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -369,7 +383,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,6 +428,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,11 +440,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,24 +460,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -541,22 +567,22 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.7627906976744"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="26" min="9" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="26" min="9" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="13.046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -738,84 +764,96 @@
         <v>36</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="C9" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -853,44 +891,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="26" min="6" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="26" min="6" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="13.046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -898,7 +936,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -915,296 +953,366 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="F4" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="H4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="J4" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="K4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="L4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="M4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="N4" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="O4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="18" t="n">
+      <c r="B5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="18" t="n">
+      <c r="E6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" s="21"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="20" t="n">
+      <c r="E7" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="P7" s="21"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="18" t="n">
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="P8" s="21"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="18" t="n">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="H5" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="18" t="n">
+      <c r="E9" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="P9" s="21"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="L5" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" s="18" t="n">
+      <c r="E10" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="P10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="24" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="18" t="n">
-        <v>5</v>
-      </c>
-      <c r="P5" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-    </row>
-    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-    </row>
-    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-    </row>
-    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
-        <v>5</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-    </row>
-    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="F11" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="n">
+      <c r="A12" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
+      <c r="A13" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>